<commit_message>
feat: Add power end analysis
creates same email for power end trend as fluid end
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alester\Desktop\Daily_KCF_Report_Current\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Desktop\React Nanodegree\MyReads Project\myreads\Daily_KCF_Report_Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1325401D-DEA2-4DB6-94B3-D35F81FB2977}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="emails" sheetId="1" r:id="rId1"/>
@@ -21,21 +22,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
-    <t>Marco Carmona &lt;Marco.Carmona@ftsi.com&gt;; Raul Galvan-Kalinchuk &lt;Raul.Galvan-Kalinchuk@ftsi.com&gt;; John Barrera &lt;John.Barrera@ftsi.com&gt;; Gustavo Machuca &lt;Gustavo.Machuca@ftsi.com&gt;; Daniel Carrera &lt;Daniel.Carrera@ftsi.com&gt;; Miguel Zuniga &lt;Miguel.Zuniga@ftsi.com&gt;; Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;</t>
-  </si>
-  <si>
     <t>Jose Rodriguez &lt;Jose.Rodriguez5@ftsi.com&gt;; Jay Crawford &lt;Jay.Crawford@ftsi.com&gt;; Clark Akers &lt;Clark.Akers@ftsi.com&gt;; Saul Lopez &lt;Saul.Lopez@ftsi.com&gt;; Gerardo Salinas &lt;Gerardo.Salinas@ftsi.com&gt;; Angel Alvarado &lt;Angel.Alvarado@ftsi.com&gt;, Jose Delgado &lt;Jose.Delgado2@ftsi.com&gt;, Max Taylor &lt;Max.Taylor@ftsi.com&gt;</t>
   </si>
   <si>
-    <t>James Demoss &lt;James.Demoss@ftsi.com&gt;; Cody Irwin &lt;Cody.Irwin@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; KCF Tech &lt;sentryftsi@kcftech.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;</t>
-  </si>
-  <si>
     <t>Ivan Presas &lt;Ivan.Presas@ftsi.com&gt;; John Carter &lt;John.Carter@ftsi.com&gt;; Justin Tamplin &lt;Justin.Tamplin@ftsi.com&gt;; Ismael Soto &lt;Ismael.Soto@ftsi.com&gt;; Mulifalaula Lealaitafea &lt;Mulifalaula.Lealaitafea@ftsi.com&gt;</t>
   </si>
   <si>
-    <t>Lencho Renteria &lt;Lencho.Renteria@ftsi.com&gt;; Jesus Garcia &lt;Jesus.Garcia@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Briar Taylor &lt;Briar.Taylor@ftsi.com&gt;; Adel Kanaan &lt;Adel.Kanaan@ftsi.com&gt;; Shamni Velayutham &lt;Shamni.Velayutham@ftsi.com&gt;; Mohammed Barakat &lt;Mohammed.Barakat@ftsi.com&gt;;Taylor Ennis &lt;Taylor.Ennis@ftsi.com&gt;;Adan.Cardona@ftsi.com</t>
-  </si>
-  <si>
     <t>Anthony Brazell &lt;Anthony.Brazell@ftsi.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Jesus Castro &lt;Jesus.Castro@ftsi.com&gt;; Juan Olazaba &lt;Juan.Olazaba@ftsi.com&gt;; Brandon Slaton &lt;Brandon.Slaton@ftsi.com&gt;; Byron Austin &lt;Byron.Austin@ftsi.com&gt;; John Demoss &lt;John.Demoss@ftsi.com&gt;; Ryan Castillo &lt;Ryan.Castillo@ftsi.com&gt;; Michael Driver &lt;Michael.Driver@ftsi.com&gt;; Nicholas Perez-Lasala &lt;Nicholas.Perez@ftsi.com&gt;</t>
   </si>
   <si>
@@ -45,28 +37,37 @@
     <t>Fernando Segovia &lt;Fernando.Segovia@ftsi.com&gt;; Alfredo Olmos &lt;Alfredo.Olmos@ftsi.com&gt;; Roberto Rivera &lt;Roberto.Rivera@ftsi.com&gt;; Jesus Barrera &lt;Jesus.Barrera2@ftsi.com&gt;; Brandon Palma &lt;Brandon.Palma@ftsi.com&gt;; Ismael Soto &lt;Ismael.Soto@ftsi.com&gt;; 'Flavio Bombonato' &lt;fbombonato@kcftech.com&gt;; Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;;Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;;Hector Hinostroza &lt;Hector.Hinostroza@ftsi.com&gt;</t>
   </si>
   <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; 'Flavio Bombonato' &lt;fbombonato@kcftech.com&gt;; tbritton@kcftech.com;Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;; Charles Hale &lt;Charles.Hale@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Timothy Johnson &lt;Timothy.Johnson@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Donovan Denmon &lt;Donovan.Denmon@ftsi.com&gt;; Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Tyler Phillips &lt;Tyler.Phillips@ftsi.com&gt;; Ezhi Subramanian &lt;Ezhi.Subramanian@ftsi.com&gt;; Hector Hinostroza &lt;Hector.Hinostroza@ftsi.com&gt;; Jeremy Grissom &lt;Jeremy.Grissom@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; 'Flavio Bombonato' &lt;fbombonato@kcftech.com&gt;; Mmeri Emeji &lt;Mmeri.Emeji@ftsi.com&gt;; Omar Saleh &lt;Omar.Saleh@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>John Romiluyi &lt;John.Romiluyi@ftsi.com&gt;; Jerrod Olmstead &lt;Jerrod.Olmstead@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Hussein Aydi &lt;Hussein.Aydi@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;</t>
-  </si>
-  <si>
     <t>Dedron Sells &lt;Dedron.Sells@ftsi.com&gt;; Joseph Esposito &lt;Joseph.Esposito@ftsi.com&gt;; John Demoss &lt;John.Demoss@ftsi.com&gt;;Saul Martinez &lt;Saul.Martinez@ftsi.com&gt;;Briar Taylor &lt;Briar.Taylor@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; 'Flavio Bombonato' &lt;fbombonato@kcftech.com&gt;; tbritton@kcftech.com;Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;; Charles Hale &lt;Charles.Hale@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>John Romiluyi &lt;John.Romiluyi@ftsi.com&gt;; Jerrod Olmstead &lt;Jerrod.Olmstead@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Hussein Aydi &lt;Hussein.Aydi@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Timothy Johnson &lt;Timothy.Johnson@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>James Demoss &lt;James.Demoss@ftsi.com&gt;; Cody Irwin &lt;Cody.Irwin@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; KCF Tech &lt;sentryftsi@kcftech.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Donovan Denmon &lt;Donovan.Denmon@ftsi.com&gt;; Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Tyler Phillips &lt;Tyler.Phillips@ftsi.com&gt;; Ezhi Subramanian &lt;Ezhi.Subramanian@ftsi.com&gt;; Hector Hinostroza &lt;Hector.Hinostroza@ftsi.com&gt;; Jeremy Grissom &lt;Jeremy.Grissom@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Lencho Renteria &lt;Lencho.Renteria@ftsi.com&gt;; Jesus Garcia &lt;Jesus.Garcia@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Briar Taylor &lt;Briar.Taylor@ftsi.com&gt;; Adel Kanaan &lt;Adel.Kanaan@ftsi.com&gt;; Shamni Velayutham &lt;Shamni.Velayutham@ftsi.com&gt;; Mohammed Barakat &lt;Mohammed.Barakat@ftsi.com&gt;;Taylor Ennis &lt;Taylor.Ennis@ftsi.com&gt;;Adan.Cardona@ftsi.com;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Marco Carmona &lt;Marco.Carmona@ftsi.com&gt;; Raul Galvan-Kalinchuk &lt;Raul.Galvan-Kalinchuk@ftsi.com&gt;;Gustavo Machuca &lt;Gustavo.Machuca@ftsi.com&gt;; Daniel Carrera &lt;Daniel.Carrera@ftsi.com&gt;; Miguel Zuniga &lt;Miguel.Zuniga@ftsi.com&gt;; Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; 'Flavio Bombonato' &lt;fbombonato@kcftech.com&gt;; Mmeri Emeji &lt;Mmeri.Emeji@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -898,68 +899,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
@@ -969,12 +970,12 @@
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exclude mislabelled green pumps for now
</commit_message>
<xml_diff>
--- a/emails.xlsx
+++ b/emails.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\austi\Desktop\React Nanodegree\MyReads Project\myreads\Daily_KCF_Report_Current\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6FD4D4E-669D-419B-9892-8A07517C8839}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3854F60A-1D8B-41E9-A0A4-71FC3866FE0F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="7470" windowHeight="2160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="11">
   <si>
     <t>Ivan Presas &lt;Ivan.Presas@ftsi.com&gt;; John Carter &lt;John.Carter@ftsi.com&gt;; Justin Tamplin &lt;Justin.Tamplin@ftsi.com&gt;; Ismael Soto &lt;Ismael.Soto@ftsi.com&gt;; Mulifalaula Lealaitafea &lt;Mulifalaula.Lealaitafea@ftsi.com&gt;</t>
   </si>
@@ -28,40 +28,31 @@
     <t>Lencho Renteria &lt;Lencho.Renteria@ftsi.com&gt;; Jesus Garcia &lt;Jesus.Garcia@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Briar Taylor &lt;Briar.Taylor@ftsi.com&gt;; Adel Kanaan &lt;Adel.Kanaan@ftsi.com&gt;; Shamni Velayutham &lt;Shamni.Velayutham@ftsi.com&gt;; Mohammed Barakat &lt;Mohammed.Barakat@ftsi.com&gt;;Taylor Ennis &lt;Taylor.Ennis@ftsi.com&gt;;Adan.Cardona@ftsi.com;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;</t>
   </si>
   <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; tbritton@kcftech.com;Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;; Charles Hale &lt;Charles.Hale@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>John Romiluyi &lt;John.Romiluyi@ftsi.com&gt;; Jerrod Olmstead &lt;Jerrod.Olmstead@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Hussein Aydi &lt;Hussein.Aydi@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;;tbritton@kcftech.com;</t>
-  </si>
-  <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Timothy Johnson &lt;Timothy.Johnson@ftsi.com&gt;; tbritton@kcftech.com; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;;  Mmeri Emeji &lt;Mmeri.Emeji@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;;tbritton@kcftech.com;</t>
-  </si>
-  <si>
-    <t>Marco Carmona &lt;Marco.Carmona@ftsi.com&gt;; Raul Galvan-Kalinchuk &lt;Raul.Galvan-Kalinchuk@ftsi.com&gt;;Gustavo Machuca &lt;Gustavo.Machuca@ftsi.com&gt;; Miguel Zuniga &lt;Miguel.Zuniga@ftsi.com&gt;;Brandon Lowrey &lt;Brandon.Lowrey@ftsi.com&gt;;Dave Perkins &lt;Dave.Perkins@ftsi.com&gt;; Jose Martinez &lt;Jose.Martinez2@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>John Demoss &lt;John.Demoss@ftsi.com&gt;;Saul Martinez &lt;Saul.Martinez@ftsi.com&gt;;Briar Taylor &lt;Briar.Taylor@ftsi.com&gt;;Jose Santos &lt;Jose.Santos@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Anthony Brazell &lt;Anthony.Brazell@ftsi.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Jesus Castro &lt;Jesus.Castro@ftsi.com&gt;; Juan Olazaba &lt;Juan.Olazaba@ftsi.com&gt;; Brandon Slaton &lt;Brandon.Slaton@ftsi.com&gt;; Byron Austin &lt;Byron.Austin@ftsi.com&gt;; John Demoss &lt;John.Demoss@ftsi.com&gt;; Ryan Castillo &lt;Ryan.Castillo@ftsi.com&gt;; Michael Driver &lt;Michael.Driver@ftsi.com&gt;; Nicholas Perez-Lasala &lt;Nicholas.Perez@ftsi.com&gt;;Aaron Getgen &lt;Aaron.Getgen@ftsi.com&gt;</t>
-  </si>
-  <si>
     <t>Jose Rodriguez &lt;Jose.Rodriguez5@ftsi.com&gt;; Jay Crawford &lt;Jay.Crawford@ftsi.com&gt;; Clark Akers &lt;Clark.Akers@ftsi.com&gt;; Saul Lopez &lt;Saul.Lopez@ftsi.com&gt;; Gerardo Salinas &lt;Gerardo.Salinas@ftsi.com&gt;; Angel Alvarado &lt;Angel.Alvarado@ftsi.com&gt;, Jose Delgado &lt;Jose.Delgado2@ftsi.com&gt;, Max Taylor &lt;Max.Taylor@ftsi.com&gt;;William Blunk &lt;William.Blunk@ftsi.com&gt;</t>
   </si>
   <si>
     <t>Cody Irwin &lt;Cody.Irwin@ftsi.com&gt;; Flavio Bombonato &lt;fbombonato@kcftech.com&gt;; KCF Tech &lt;sentryftsi@kcftech.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;</t>
   </si>
   <si>
-    <t>Donovan Denmon &lt;Donovan.Denmon@ftsi.com&gt;; Jonathan Woodson &lt;Jonathan.Woodson@ftsi.com&gt;; Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Tyler Phillips &lt;Tyler.Phillips@ftsi.com&gt;; Ezhi Subramanian &lt;Ezhi.Subramanian@ftsi.com&gt;; Hector Hinostroza &lt;Hector.Hinostroza@ftsi.com&gt;; Jeremy Grissom &lt;Jeremy.Grissom@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;;Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;;Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;;tbritton@kcftech.com;</t>
-  </si>
-  <si>
-    <t>Dedron Sells &lt;Dedron.Sells@ftsi.com&gt;; Joseph Esposito &lt;Joseph.Esposito@ftsi.com&gt;;Richard Mears &lt;Richard.Mears@ftsi.com&gt;; Sergio Rodarte &lt;Sergio.Rodarte@ftsi.com&gt;; Samuel Campos &lt;Samuel.Campos@ftsi.com&gt;; Charles Hale &lt;Charles.Hale@ftsi.com&gt;; Andre Malone &lt;Andre.Malone@ftsi.com&gt;;William Blunk &lt;William.Blunk@ftsi.com&gt;;Jay Grooms &lt;Jay.Grooms@ftsi.com&gt;;Chad Clement &lt;Chad.Clement@ftsi.com&gt;</t>
-  </si>
-  <si>
-    <t>Fernando Segovia &lt;Fernando.Segovia@ftsi.com&gt;; Alfredo Olmos &lt;Alfredo.Olmos@ftsi.com&gt;; Roberto Rivera &lt;Roberto.Rivera@ftsi.com&gt;; Jesus Barrera &lt;Jesus.Barrera2@ftsi.com&gt;; Ismael Soto &lt;Ismael.Soto@ftsi.com&gt;;  Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;;Hector Hinostroza &lt;Hector.Hinostroza@ftsi.com&gt;; Ryan Castillo &lt;Ryan.Castillo@ftsi.com&gt;;Jeremy Grissom &lt;Jeremy.Grissom@ftsi.com&gt;</t>
+    <t>Kevin Roycroft &lt;Kevin.Roycroft@ftsi.com&gt;; Saul Martinez &lt;Saul.Martinez@ftsi.com&gt;; Issac Jacquez &lt;Issac.Jacquez@ftsi.com&gt;; Andre Malone &lt;Andre.Malone@ftsi.com&gt;; Charles Hale &lt;Charles.Hale@ftsi.com&gt;; James Demoss &lt;James.Demoss@ftsi.com&gt;; Jose Santos &lt;Jose.Santos@ftsi.com&gt;; Ziad Kanaan &lt;Ziad.Kanaan@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Teddy Woodson &lt;Teddy.Woodson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;; Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;; 'tbritton@kcftech.com'; Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Dedron Sells &lt;Dedron.Sells@ftsi.com&gt;; Joseph Esposito &lt;Joseph.Esposito@ftsi.com&gt;; Joshua Haynes &lt;Joshua.Haynes@ftsi.com&gt;; John Romiluyi &lt;John.Romiluyi@ftsi.com&gt;; Sammy Campos &lt;Samuel.Campos@ftsi.com&gt;; Mohammed Barakat &lt;Mohammed.Barakat@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Max Taylor &lt;Max.Taylor@ftsi.com&gt;; Teddy Woodson &lt;Teddy.Woodson@ftsi.com&gt;; Daniel Jones &lt;Daniel.Jones3@ftsi.com&gt;; Willie Atkinson &lt;Willie.Atkinson@ftsi.com&gt;; Odessa Technical Advisors &lt;OdessaTechAdvisors@ftsi.com&gt;; tbritton@kcftech.com; Richard Bushnell &lt;Richard.Bushnell@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Raul Galvan-Kalinchuk &lt;Raul.Galvan-Kalinchuk@ftsi.com&gt;; Alberto Ortiz &lt;Alberto.Ortiz@ftsi.com&gt;; Gustavo Machuca &lt;Gustavo.Machuca@ftsi.com&gt;; Jose Quintanilla &lt;Jose.Quintanilla@ftsi.com&gt;; Miguel Zuniga &lt;Miguel.Zuniga@ftsi.com&gt;; Marco Carmona &lt;Marco.Carmona@ftsi.com&gt;; Brandon Lowrey &lt;Brandon.Lowrey@ftsi.com&gt;; Dave Perkins &lt;Dave.Perkins@ftsi.com&gt;; Jose Martinez &lt;Jose.Martinez2@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Byron Austin &lt;Byron.Austin@ftsi.com&gt;; Hussein Aydi &lt;Hussein.Aydi@ftsi.com&gt;; Jesus Castro &lt;Jesus.Castro@ftsi.com&gt;; Juan Olazaba &lt;Juan.Olazaba@ftsi.com&gt;; Brandon Slaton &lt;Brandon.Slaton@ftsi.com&gt;; Nicholas Perez-Lasala &lt;Nicholas.Perez@ftsi.com&gt;; Michael Driver &lt;Michael.Driver@ftsi.com&gt;; Aaron Getgen &lt;Aaron.Getgen@ftsi.com&gt;; John Demoss &lt;John.Demoss@ftsi.com&gt;</t>
+  </si>
+  <si>
+    <t>Luis Salinas &lt;Luis.Salinas@ftsi.com&gt;; Fernando Segovia &lt;Fernando.Segovia@ftsi.com&gt;; Roberto Rivera &lt;Roberto.Rivera@ftsi.com&gt;; Jesus Barrera &lt;Jesus.Barrera2@ftsi.com&gt;; Ismael Soto &lt;Ismael.Soto@ftsi.com&gt;; Jeremy Grissom &lt;Jeremy.Grissom@ftsi.com&gt;; Ryan Castillo &lt;Ryan.Castillo@ftsi.com&gt;; Donovan Denmon &lt;Donovan.Denmon@ftsi.com&gt;</t>
   </si>
 </sst>
 </file>
@@ -903,34 +894,34 @@
   <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -940,32 +931,32 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>